<commit_message>
made for biometric reports
</commit_message>
<xml_diff>
--- a/outputs/leave_records_report.xlsx
+++ b/outputs/leave_records_report.xlsx
@@ -33,12 +33,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -68,11 +74,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,117 +454,163 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>COUNT</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Leave Report</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Leave Report</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 1</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 2</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 3</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 6</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 7</t>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Department: SURVEYOR</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+      <c r="F2" s="2" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Department: SURVEYOR</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>1321</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>ABDALLAH IBRAHIMU</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>ABDALLAH</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>SURVEYOR</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1321</t>
+          <t>1347</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ABDALLAH IBRAHIMU</t>
+          <t>WILLIAM JAMES</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ABDALLAH</t>
+          <t>MARWA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -567,7 +620,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SURVEYOR</t>
+          <t>CHIEF SURVEYOR</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -589,141 +642,122 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1347</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>WILLIAM JAMES</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>MARWA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>CHIEF SURVEYOR</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
           <t>10.0</t>
         </is>
       </c>
     </row>
-    <row r="8"/>
+    <row r="7"/>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Department: STORE</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" s="2" t="n"/>
+      <c r="G8" s="2" t="n"/>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
+        </is>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Department: STORE</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>FABIAN EDWARD</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>NJAHASI</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>TRACTOR OPERATOR-LOW HP</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FABIAN EDWARD</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>NJAHASI</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TRACTOR OPERATOR-LOW HP</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -732,102 +766,113 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Department: IRRIGATION</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
+        </is>
+      </c>
+    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Department: IRRIGATION</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>938</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>HERI LADISLAUS</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>LUANDE</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>IRRIGATION ENGINEER</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>938</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HERI LADISLAUS</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>LUANDE</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>IRRIGATION ENGINEER</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -836,102 +881,113 @@
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="18"/>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Department: HUMAN RESOURCES</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
+      <c r="H18" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
+        </is>
+      </c>
+    </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Department: HUMAN RESOURCES</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>2818</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>SAMWEL GEORGE</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>ARON</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>LAWYER</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2818</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SAMWEL GEORGE</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ARON</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LAWYER</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -940,102 +996,113 @@
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23"/>
+    <row r="22"/>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Department: SHEQ</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="n"/>
+      <c r="E23" s="2" t="n"/>
+      <c r="F23" s="2" t="n"/>
+      <c r="G23" s="2" t="n"/>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
+        </is>
+      </c>
+    </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Department: SHEQ</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>2910</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>LINETH FIDEL</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>OWINO</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>SAFETY OFFICER</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2910</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LINETH FIDEL</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>OWINO</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>SAFETY OFFICER</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1044,117 +1111,116 @@
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="28"/>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Department: CIVIL</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="n"/>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>Count: 0</t>
+        </is>
+      </c>
+    </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Department: CIVIL</t>
+          <t>Employee ID</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Weekday</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Annual Leave(H)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Employee ID</t>
+          <t>2748</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>ELIFURAHA ELIHAKI</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>MNZAVA</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>M</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>DATA CLERK</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>2025-09-13</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Weekday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Annual Leave(H)</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2748</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>ELIFURAHA ELIHAKI</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>MNZAVA</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>DATA CLERK</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>2025-09-13</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Saturday</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Statistics</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
         <is>
           <t>5.0</t>
         </is>

</xml_diff>